<commit_message>
Created html file for plots for better interactivity
</commit_message>
<xml_diff>
--- a/src/MADS_Runtime.xlsx
+++ b/src/MADS_Runtime.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:A121"/>
+  <dimension ref="A1:A81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,602 +392,402 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.1959998607635498</v>
+        <v>0.2590000629425049</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.08800005912780762</v>
+        <v>0.14599990844726562</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>0.07700014114379883</v>
+        <v>0.11400008201599121</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>0.06800007820129395</v>
+        <v>0.10400009155273438</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>0.06200003623962402</v>
+        <v>0.11599993705749512</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0.0690000057220459</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>0.08800005912780762</v>
+        <v>0.09400010108947754</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>0.06200003623962402</v>
+        <v>0.08599996566772461</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>0.06399989128112793</v>
+        <v>0.09299993515014648</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>0.11599993705749512</v>
+        <v>0.08700013160705566</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>0.1679999828338623</v>
+        <v>0.1119999885559082</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>0.07200002670288086</v>
+        <v>0.08999991416931152</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>0.06699991226196289</v>
+        <v>0.08599996566772461</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>0.07000017166137695</v>
+        <v>0.08099985122680664</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>0.0690000057220459</v>
+        <v>0.07500004768371582</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>0.06599998474121094</v>
+        <v>0.10400009155273438</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>0.07399988174438477</v>
+        <v>0.10400009155273438</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>0.06599998474121094</v>
+        <v>0.15000009536743164</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>0.09100008010864258</v>
+        <v>0.1510000228881836</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>0.0840001106262207</v>
+        <v>0.10400009155273438</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>0.09500002861022949</v>
+        <v>0.0839998722076416</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>0.08699989318847656</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>0.08099985122680664</v>
+        <v>0.1119999885559082</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>0.1099998950958252</v>
+        <v>0.0969998836517334</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>0.09100008010864258</v>
+        <v>0.11500000953674316</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>0.10300016403198242</v>
+        <v>0.08500003814697266</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>0.08800005912780762</v>
+        <v>0.09999990463256836</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>0.09200000762939453</v>
+        <v>0.07399988174438477</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>0.08600020408630371</v>
+        <v>0.07500004768371582</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>0.07599997520446777</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>0.08300018310546875</v>
+        <v>0.0970001220703125</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>0.0820000171661377</v>
+        <v>0.09099984169006348</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>0.08299994468688965</v>
+        <v>0.10000014305114746</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>0.07699990272521973</v>
+        <v>0.08699989318847656</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>0.07200002670288086</v>
+        <v>0.0839998722076416</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>0.07200002670288086</v>
+        <v>0.08599996566772461</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>0.08899998664855957</v>
+        <v>0.09800004959106445</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>0.08100008964538574</v>
+        <v>0.0969998836517334</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>0.11299991607666016</v>
+        <v>0.0989999771118164</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>0.11100006103515625</v>
+        <v>0.0820000171661377</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>0.22499990463256836</v>
+        <v>0.08699989318847656</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>0.22099995613098145</v>
+        <v>0.10100007057189941</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>0.24200010299682617</v>
+        <v>0.09199976921081543</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>0.24599981307983398</v>
+        <v>0.0820000171661377</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>0.14899992942810059</v>
+        <v>0.07999992370605469</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>0.1679999828338623</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>0.18700003623962402</v>
+        <v>0.11100006103515625</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>0.27899980545043945</v>
+        <v>0.11999988555908203</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>0.20199990272521973</v>
+        <v>0.11999988555908203</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>0.2650001049041748</v>
+        <v>0.11899995803833008</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>0.2569999694824219</v>
+        <v>0.11500000953674316</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>0.28600001335144043</v>
+        <v>0.10299992561340332</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>0.12899994850158691</v>
+        <v>0.1119999885559082</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>0.13300013542175293</v>
+        <v>0.09399986267089844</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>0.1700000762939453</v>
+        <v>0.1359999179840088</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>0.17800021171569824</v>
+        <v>0.0840001106262207</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>0.13300013542175293</v>
+        <v>0.0970001220703125</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>0.1639997959136963</v>
+        <v>0.08899998664855957</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>0.18700003623962402</v>
+        <v>0.08700013160705566</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>0.20799994468688965</v>
+        <v>0.08299994468688965</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>0.12100005149841309</v>
+        <v>0.08000016212463379</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>0.14499998092651367</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>0.16199994087219238</v>
+        <v>0.09299993515014648</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>0.19300007820129395</v>
+        <v>0.0969998836517334</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>0.14700007438659668</v>
+        <v>0.0840001106262207</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>0.21199989318847656</v>
+        <v>0.08899998664855957</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>0.31999993324279785</v>
+        <v>0.08500003814697266</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>0.28099989891052246</v>
+        <v>0.09299993515014648</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>0.10300016403198242</v>
+        <v>0.08799982070922852</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>0.12800002098083496</v>
+        <v>0.08500003814697266</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>0.16300010681152344</v>
+        <v>0.10500001907348633</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>0.16900014877319336</v>
+        <v>0.08099985122680664</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>0.20000004768371582</v>
+        <v>0.06999993324279785</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>0.2070000171661377</v>
+        <v>0.08700013160705566</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>0.27300000190734863</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>0.3039999008178711</v>
+        <v>0.0970001220703125</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
-        <v>0.10500001907348633</v>
+        <v>0.09399986267089844</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <v>0.16499996185302734</v>
+        <v>0.10500001907348633</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>0.18400001525878906</v>
+        <v>0.09099984169006348</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
-        <v>0.1940000057220459</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82">
-        <v>0.18899989128112793</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83">
-        <v>0.17199993133544922</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84">
-        <v>0.17400002479553223</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85">
-        <v>0.23000001907348633</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86">
-        <v>0.17399978637695312</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87">
-        <v>0.26199984550476074</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88">
-        <v>0.29799985885620117</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89">
-        <v>0.21799993515014648</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90">
-        <v>0.1510000228881836</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91">
-        <v>0.2050001621246338</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92">
-        <v>0.18399977684020996</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93">
-        <v>0.20199990272521973</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94">
-        <v>0.12199997901916504</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95">
-        <v>0.12999987602233887</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96">
-        <v>0.13100004196166992</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97">
-        <v>0.1660001277923584</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98">
-        <v>0.12899994850158691</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99">
-        <v>0.1510000228881836</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100">
-        <v>0.17300009727478027</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101">
-        <v>0.2669999599456787</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102">
-        <v>0.17199993133544922</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103">
-        <v>0.3340001106262207</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104">
-        <v>0.11100006103515625</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105">
-        <v>0.34400010108947754</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106">
-        <v>0.13199996948242188</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107">
-        <v>0.1230001449584961</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108">
-        <v>0.11800003051757812</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109">
-        <v>0.11899995803833008</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110">
-        <v>0.1490001678466797</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111">
-        <v>0.2910001277923584</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112">
-        <v>0.31800007820129395</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113">
-        <v>0.26200008392333984</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114">
-        <v>0.22800016403198242</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115">
-        <v>0.2949998378753662</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116">
-        <v>0.25999999046325684</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117">
-        <v>0.2110002040863037</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118">
-        <v>0.12800002098083496</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119">
-        <v>0.16900014877319336</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120">
-        <v>0.2330000400543213</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121">
-        <v>0.2990000247955322</v>
+        <v>0.08999991416931152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Application of safety margins for collision avoidance
</commit_message>
<xml_diff>
--- a/src/MADS_Runtime.xlsx
+++ b/src/MADS_Runtime.xlsx
@@ -392,402 +392,402 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.2590000629425049</v>
+        <v>0.7889997959136963</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.14599990844726562</v>
+        <v>0.13100004196166992</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>0.11400008201599121</v>
+        <v>0.15399980545043945</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>0.10400009155273438</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>0.11599993705749512</v>
+        <v>0.0839998722076416</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0.09599995613098145</v>
+        <v>0.0840001106262207</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>0.09400010108947754</v>
+        <v>0.09800004959106445</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>0.08599996566772461</v>
+        <v>0.11100006103515625</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>0.09299993515014648</v>
+        <v>0.09100008010864258</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>0.08700013160705566</v>
+        <v>0.09500002861022949</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>0.1119999885559082</v>
+        <v>0.08699989318847656</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>0.08999991416931152</v>
+        <v>0.09099984169006348</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>0.08599996566772461</v>
+        <v>0.1119999885559082</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>0.08099985122680664</v>
+        <v>0.10899996757507324</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>0.07500004768371582</v>
+        <v>0.10100007057189941</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>0.10400009155273438</v>
+        <v>0.09400010108947754</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>0.10400009155273438</v>
+        <v>0.0820000171661377</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>0.15000009536743164</v>
+        <v>0.08999991416931152</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>0.1510000228881836</v>
+        <v>0.08499979972839355</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>0.10400009155273438</v>
+        <v>0.12400007247924805</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>0.0839998722076416</v>
+        <v>0.1119999885559082</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>0.09200000762939453</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>0.1119999885559082</v>
+        <v>0.09300017356872559</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>0.0969998836517334</v>
+        <v>0.08300018310546875</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>0.11500000953674316</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>0.08500003814697266</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>0.09999990463256836</v>
+        <v>0.10299992561340332</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>0.07399988174438477</v>
+        <v>0.15899991989135742</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>0.07500004768371582</v>
+        <v>0.11800003051757812</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>0.09200000762939453</v>
+        <v>0.1119999885559082</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>0.0970001220703125</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>0.09099984169006348</v>
+        <v>0.08100008964538574</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>0.10000014305114746</v>
+        <v>0.0840001106262207</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>0.08699989318847656</v>
+        <v>0.0989999771118164</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>0.0839998722076416</v>
+        <v>0.08699989318847656</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>0.08599996566772461</v>
+        <v>0.08299994468688965</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>0.09800004959106445</v>
+        <v>0.09599995613098145</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>0.0969998836517334</v>
+        <v>0.09299993515014648</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>0.0989999771118164</v>
+        <v>0.11299991607666016</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>0.0820000171661377</v>
+        <v>0.08299994468688965</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>0.08699989318847656</v>
+        <v>0.11599993705749512</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>0.10100007057189941</v>
+        <v>0.09400010108947754</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>0.09199976921081543</v>
+        <v>0.10100007057189941</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>0.0820000171661377</v>
+        <v>0.08799982070922852</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>0.07999992370605469</v>
+        <v>0.11299991607666016</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>0.09599995613098145</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>0.11100006103515625</v>
+        <v>0.10300016403198242</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>0.11999988555908203</v>
+        <v>0.08699989318847656</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>0.11999988555908203</v>
+        <v>0.08100008964538574</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>0.11899995803833008</v>
+        <v>0.11399984359741211</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>0.11500000953674316</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>0.10299992561340332</v>
+        <v>0.09600019454956055</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>0.1119999885559082</v>
+        <v>0.09100008010864258</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>0.09399986267089844</v>
+        <v>0.08800005912780762</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>0.1359999179840088</v>
+        <v>0.0970001220703125</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>0.0840001106262207</v>
+        <v>0.11100006103515625</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>0.0970001220703125</v>
+        <v>0.10000014305114746</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>0.08899998664855957</v>
+        <v>0.09100008010864258</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>0.08700013160705566</v>
+        <v>0.0970001220703125</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>0.08299994468688965</v>
+        <v>0.08500003814697266</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>0.08000016212463379</v>
+        <v>0.09399986267089844</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>0.09599995613098145</v>
+        <v>0.10800004005432129</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>0.09299993515014648</v>
+        <v>0.10699987411499023</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>0.0969998836517334</v>
+        <v>0.08700013160705566</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>0.0840001106262207</v>
+        <v>0.08599996566772461</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>0.08899998664855957</v>
+        <v>0.0820000171661377</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>0.08500003814697266</v>
+        <v>0.09400010108947754</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>0.09299993515014648</v>
+        <v>0.1099998950958252</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>0.08799982070922852</v>
+        <v>0.0839998722076416</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>0.08500003814697266</v>
+        <v>0.10199999809265137</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>0.10500001907348633</v>
+        <v>0.0989999771118164</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>0.08099985122680664</v>
+        <v>0.09099984169006348</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>0.06999993324279785</v>
+        <v>0.09400010108947754</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>0.08700013160705566</v>
+        <v>0.08999991416931152</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>0.09599995613098145</v>
+        <v>0.10500001907348633</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>0.0970001220703125</v>
+        <v>0.08600020408630371</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
-        <v>0.09399986267089844</v>
+        <v>0.07999992370605469</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <v>0.10500001907348633</v>
+        <v>0.07899999618530273</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>0.09099984169006348</v>
+        <v>0.0969998836517334</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
-        <v>0.08999991416931152</v>
+        <v>0.09800004959106445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added area coverage plots on top of fire propagation plot
</commit_message>
<xml_diff>
--- a/src/MADS_Runtime.xlsx
+++ b/src/MADS_Runtime.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:A81"/>
+  <dimension ref="A1:A121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,402 +392,602 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.7889997959136963</v>
+        <v>0.26600003242492676</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.13100004196166992</v>
+        <v>0.13200020790100098</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>0.15399980545043945</v>
+        <v>0.06400012969970703</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>0.09200000762939453</v>
+        <v>0.05500006675720215</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>0.0839998722076416</v>
+        <v>0.048999786376953125</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0.0840001106262207</v>
+        <v>0.05900001525878906</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>0.09800004959106445</v>
+        <v>0.05200004577636719</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>0.11100006103515625</v>
+        <v>0.05900001525878906</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>0.09100008010864258</v>
+        <v>0.06299996376037598</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>0.09500002861022949</v>
+        <v>0.05200004577636719</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>0.08699989318847656</v>
+        <v>0.06100010871887207</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>0.09099984169006348</v>
+        <v>0.10099983215332031</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>0.1119999885559082</v>
+        <v>0.06599998474121094</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>0.10899996757507324</v>
+        <v>0.059999942779541016</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>0.10100007057189941</v>
+        <v>0.06200003623962402</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>0.09400010108947754</v>
+        <v>0.06600022315979004</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>0.0820000171661377</v>
+        <v>0.05299997329711914</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>0.08999991416931152</v>
+        <v>0.06500005722045898</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>0.08499979972839355</v>
+        <v>0.059999942779541016</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>0.12400007247924805</v>
+        <v>0.054000139236450195</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>0.1119999885559082</v>
+        <v>0.06399989128112793</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>0.09599995613098145</v>
+        <v>0.06200003623962402</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>0.09300017356872559</v>
+        <v>0.05800008773803711</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>0.08300018310546875</v>
+        <v>0.06500005722045898</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>0.09599995613098145</v>
+        <v>0.11299991607666016</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>0.09200000762939453</v>
+        <v>0.06599998474121094</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>0.10299992561340332</v>
+        <v>0.06000018119812012</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>0.15899991989135742</v>
+        <v>0.059999942779541016</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>0.11800003051757812</v>
+        <v>0.059999942779541016</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>0.1119999885559082</v>
+        <v>0.0559999942779541</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>0.09599995613098145</v>
+        <v>0.06200003623962402</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>0.08100008964538574</v>
+        <v>0.06299996376037598</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>0.0840001106262207</v>
+        <v>0.07500004768371582</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>0.0989999771118164</v>
+        <v>0.06299996376037598</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>0.08699989318847656</v>
+        <v>0.06000018119812012</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>0.08299994468688965</v>
+        <v>0.06599998474121094</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>0.09599995613098145</v>
+        <v>0.054000139236450195</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>0.09299993515014648</v>
+        <v>0.06500005722045898</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>0.11299991607666016</v>
+        <v>0.06099987030029297</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>0.08299994468688965</v>
+        <v>0.06399989128112793</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>0.11599993705749512</v>
+        <v>0.0559999942779541</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>0.09400010108947754</v>
+        <v>0.06000018119812012</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>0.10100007057189941</v>
+        <v>0.07400012016296387</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>0.08799982070922852</v>
+        <v>0.06599998474121094</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>0.11299991607666016</v>
+        <v>0.06700015068054199</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>0.09200000762939453</v>
+        <v>0.05499982833862305</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>0.10300016403198242</v>
+        <v>0.06699991226196289</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>0.08699989318847656</v>
+        <v>0.06599998474121094</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>0.08100008964538574</v>
+        <v>0.06099987030029297</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>0.11399984359741211</v>
+        <v>0.06700015068054199</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>0.09200000762939453</v>
+        <v>0.07200002670288086</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>0.09600019454956055</v>
+        <v>0.06400012969970703</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>0.09100008010864258</v>
+        <v>0.056999921798706055</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>0.08800005912780762</v>
+        <v>0.06399989128112793</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>0.0970001220703125</v>
+        <v>0.06399989128112793</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>0.11100006103515625</v>
+        <v>0.06000018119812012</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>0.10000014305114746</v>
+        <v>0.07400012016296387</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>0.09100008010864258</v>
+        <v>0.07500004768371582</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>0.0970001220703125</v>
+        <v>0.06500005722045898</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>0.08500003814697266</v>
+        <v>0.07699990272521973</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>0.09399986267089844</v>
+        <v>0.07500004768371582</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>0.10800004005432129</v>
+        <v>0.09800004959106445</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>0.10699987411499023</v>
+        <v>0.06799983978271484</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>0.08700013160705566</v>
+        <v>0.07700014114379883</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>0.08599996566772461</v>
+        <v>0.0690000057220459</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>0.0820000171661377</v>
+        <v>0.07999992370605469</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>0.09400010108947754</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>0.1099998950958252</v>
+        <v>0.09200000762939453</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>0.0839998722076416</v>
+        <v>0.07899999618530273</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>0.10199999809265137</v>
+        <v>0.07299995422363281</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>0.0989999771118164</v>
+        <v>0.07699990272521973</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>0.09099984169006348</v>
+        <v>0.08099985122680664</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>0.09400010108947754</v>
+        <v>0.08499979972839355</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>0.08999991416931152</v>
+        <v>0.08000016212463379</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>0.10500001907348633</v>
+        <v>0.07400012016296387</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>0.08600020408630371</v>
+        <v>0.0820000171661377</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
-        <v>0.07999992370605469</v>
+        <v>0.11400008201599121</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <v>0.07899999618530273</v>
+        <v>0.08499979972839355</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>0.0969998836517334</v>
+        <v>0.0819997787475586</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
-        <v>0.09800004959106445</v>
+        <v>0.07599997520446777</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82">
+        <v>0.07799983024597168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83">
+        <v>0.07800006866455078</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84">
+        <v>0.07200002670288086</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85">
+        <v>0.07200002670288086</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86">
+        <v>0.13699984550476074</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87">
+        <v>0.07899999618530273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88">
+        <v>0.08500003814697266</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89">
+        <v>0.09099984169006348</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90">
+        <v>0.08299994468688965</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91">
+        <v>0.08299994468688965</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92">
+        <v>0.13200020790100098</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93">
+        <v>0.07699990272521973</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94">
+        <v>0.0839998722076416</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95">
+        <v>0.07999992370605469</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96">
+        <v>0.08800005912780762</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97">
+        <v>0.07299995422363281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98">
+        <v>0.07400012016296387</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99">
+        <v>0.09999990463256836</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100">
+        <v>0.08500003814697266</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101">
+        <v>0.0839998722076416</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102">
+        <v>0.07499980926513672</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103">
+        <v>0.09200000762939453</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104">
+        <v>0.10299992561340332</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105">
+        <v>0.0969998836517334</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106">
+        <v>0.08000016212463379</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107">
+        <v>0.0820000171661377</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108">
+        <v>0.07699990272521973</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109">
+        <v>0.10199999809265137</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110">
+        <v>0.07699990272521973</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111">
+        <v>0.07399988174438477</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112">
+        <v>0.07999992370605469</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113">
+        <v>0.09100008010864258</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114">
+        <v>0.0820000171661377</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115">
+        <v>0.07500004768371582</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116">
+        <v>0.07500004768371582</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117">
+        <v>0.07999992370605469</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118">
+        <v>0.07599997520446777</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119">
+        <v>0.07599997520446777</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120">
+        <v>0.08499979972839355</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121">
+        <v>0.09099984169006348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>